<commit_message>
add spec in quote
</commit_message>
<xml_diff>
--- a/doc/SP1 需求.xlsx
+++ b/doc/SP1 需求.xlsx
@@ -861,8 +861,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="36" spans="1:8" ht="26.4" customHeight="1">
       <c r="A36" s="26"/>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="C36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="6">
@@ -1657,7 +1657,7 @@
       <c r="F36" s="6">
         <v>2</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="18" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Spce to Sample
</commit_message>
<xml_diff>
--- a/doc/SP1 需求.xlsx
+++ b/doc/SP1 需求.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
   <si>
     <t>Page</t>
   </si>
@@ -393,6 +393,9 @@
   </si>
   <si>
     <t>SP1 修改？？</t>
+  </si>
+  <si>
+    <t>specification 字段 要在quote 的界面显示吗？？？？？</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -577,6 +580,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,8 +867,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1660,6 +1666,9 @@
       <c r="G36" s="18" t="s">
         <v>94</v>
       </c>
+      <c r="H36" s="28" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="36.6" customHeight="1">
       <c r="A37" s="26"/>
@@ -1705,13 +1714,13 @@
     </row>
     <row r="39" spans="1:8" ht="22.8" customHeight="1">
       <c r="A39" s="26"/>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="C39" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E39" s="6">
@@ -1720,7 +1729,7 @@
       <c r="F39" s="6">
         <v>1</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="18" t="s">
         <v>94</v>
       </c>
       <c r="H39" s="21" t="s">

</xml_diff>

<commit_message>
add Spce to inquiry
</commit_message>
<xml_diff>
--- a/doc/SP1 需求.xlsx
+++ b/doc/SP1 需求.xlsx
@@ -575,14 +575,14 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,7 +868,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -933,7 +933,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="27.6" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -956,7 +956,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="27.6">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
@@ -1022,7 +1022,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="34.200000000000003" customHeight="1">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="24.6" customHeight="1">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1064,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="52.8" customHeight="1">
-      <c r="A9" s="26"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="5" t="s">
         <v>55</v>
       </c>
@@ -1088,7 +1088,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" customHeight="1">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="18" t="s">
         <v>53</v>
       </c>
@@ -1109,7 +1109,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="5" t="s">
         <v>54</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" customHeight="1">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1157,7 +1157,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="29.4" customHeight="1">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="18" t="s">
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="27.6">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="18.600000000000001" customHeight="1">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="18" t="s">
         <v>17</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="24" customHeight="1">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
@@ -1243,7 +1243,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="31.2" customHeight="1">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1264,7 +1264,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.6" customHeight="1">
-      <c r="A18" s="27"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="18" t="s">
         <v>20</v>
       </c>
@@ -1285,7 +1285,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="11.4" customHeight="1">
-      <c r="A19" s="27"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="10" t="s">
         <v>21</v>
       </c>
@@ -1306,7 +1306,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.6" customHeight="1">
-      <c r="A20" s="27"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="18" t="s">
         <v>22</v>
       </c>
@@ -1327,7 +1327,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="16.8" customHeight="1">
-      <c r="A21" s="27"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1348,7 +1348,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="22.2" customHeight="1">
-      <c r="A22" s="27"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1369,7 +1369,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="13.8" customHeight="1">
-      <c r="A23" s="27"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="18" t="s">
         <v>25</v>
       </c>
@@ -1390,7 +1390,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="22.8" customHeight="1">
-      <c r="A24" s="27"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
@@ -1411,7 +1411,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="24" customHeight="1">
-      <c r="A25" s="27"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="18" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1432,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21.6" customHeight="1">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="18" t="s">
         <v>28</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="19.2" customHeight="1">
-      <c r="A27" s="27"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
@@ -1474,7 +1474,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.6" customHeight="1">
-      <c r="A28" s="27"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.6" customHeight="1">
-      <c r="A29" s="27"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="18" t="s">
         <v>31</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="82.8">
-      <c r="A30" s="27"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="8" t="s">
         <v>101</v>
       </c>
@@ -1537,7 +1537,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1">
-      <c r="A31" s="27"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="5" t="s">
         <v>32</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="21" customHeight="1">
-      <c r="A32" s="27"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="5" t="s">
         <v>33</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="27.6">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="27.6">
-      <c r="A34" s="26"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="8" t="s">
         <v>36</v>
       </c>
@@ -1626,7 +1626,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="42" customHeight="1">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1647,7 +1647,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="26.4" customHeight="1">
-      <c r="A36" s="26"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="18" t="s">
         <v>38</v>
       </c>
@@ -1666,12 +1666,12 @@
       <c r="G36" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H36" s="26" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="36.6" customHeight="1">
-      <c r="A37" s="26"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="37.799999999999997" customHeight="1">
-      <c r="A38" s="26"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="5" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="22.8" customHeight="1">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="18" t="s">
         <v>41</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="30.6" customHeight="1">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -1760,14 +1760,14 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1">
-      <c r="A41" s="26"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="27"/>
+      <c r="B41" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="C41" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E41" s="6">
@@ -1776,10 +1776,10 @@
       <c r="F41" s="6">
         <v>1</v>
       </c>
-      <c r="G41" s="4"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="26"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="8" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
modify Dept Name to required
</commit_message>
<xml_diff>
--- a/doc/SP1 需求.xlsx
+++ b/doc/SP1 需求.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="118">
   <si>
     <t>Page</t>
   </si>
@@ -374,9 +374,6 @@
     <t>按createtime排序</t>
   </si>
   <si>
-    <t>add user   Dept Name 必填项</t>
-  </si>
-  <si>
     <t>Test Method:</t>
   </si>
   <si>
@@ -396,6 +393,12 @@
   </si>
   <si>
     <t>specification 字段 要在quote 的界面显示吗？？？？？</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> post和 Dept Name 必填项</t>
   </si>
 </sst>
 </file>
@@ -867,8 +870,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1084,7 +1087,7 @@
         <v>94</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" customHeight="1">
@@ -1129,7 +1132,7 @@
         <v>94</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" customHeight="1">
@@ -1150,10 +1153,10 @@
         <v>0.2</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29.4" customHeight="1">
@@ -1557,7 +1560,7 @@
         <v>94</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="21" customHeight="1">
@@ -1667,7 +1670,7 @@
         <v>94</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="36.6" customHeight="1">
@@ -1733,7 +1736,7 @@
         <v>94</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="30.6" customHeight="1">
@@ -1843,6 +1846,9 @@
       </c>
       <c r="G44" s="18" t="s">
         <v>94</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2089,11 +2095,9 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" s="24" t="s">
-        <v>109</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B56" s="24"/>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="9"/>

</xml_diff>